<commit_message>
add some new functions problem with Jira package. Is not found
</commit_message>
<xml_diff>
--- a/jira/exmple/example.xlsx
+++ b/jira/exmple/example.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>TASK</t>
   </si>
@@ -40,6 +40,18 @@
   </si>
   <si>
     <t>про</t>
+  </si>
+  <si>
+    <t>dfsfsd</t>
+  </si>
+  <si>
+    <t>AW-13</t>
+  </si>
+  <si>
+    <t>sdsfsd</t>
+  </si>
+  <si>
+    <t>jira-3</t>
   </si>
 </sst>
 </file>
@@ -97,12 +109,12 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -389,7 +401,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -401,34 +413,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B1" s="2">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
         <v>42803</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>30</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
@@ -436,78 +449,94 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
-        <v>0</v>
+      <c r="A10" s="4">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
+      <c r="A11" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
-        <v>0</v>
-      </c>
+        <v>42804</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="5">
-        <v>0</v>
+      <c r="A13" s="4">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="5">
+      <c r="A14" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="5">
+      <c r="A15" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="5">
+      <c r="A16" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5">
+      <c r="A17" s="4">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:D1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A12:D12"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>

</xml_diff>